<commit_message>
added data to raw-population-indicator-data for Skeena rivers
</commit_message>
<xml_diff>
--- a/data/raw-population-indicator-data/CentralCoast_2006_Ptolemyetal_BellaCoola1988to2006_SS_Atnarko.xlsx
+++ b/data/raw-population-indicator-data/CentralCoast_2006_Ptolemyetal_BellaCoola1988to2006_SS_Atnarko.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8119C1-C665-4FAF-B55A-88E92B9887D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5221F6E6-3748-4257-A89C-26862BF6A47A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -492,7 +492,7 @@
         <v>683</v>
       </c>
       <c r="D2">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -536,7 +536,7 @@
         <v>683</v>
       </c>
       <c r="D3">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -580,7 +580,7 @@
         <v>683</v>
       </c>
       <c r="D4">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -624,7 +624,7 @@
         <v>683</v>
       </c>
       <c r="D5">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -668,7 +668,7 @@
         <v>683</v>
       </c>
       <c r="D6">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -712,7 +712,7 @@
         <v>683</v>
       </c>
       <c r="D7">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -756,7 +756,7 @@
         <v>683</v>
       </c>
       <c r="D8">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -800,7 +800,7 @@
         <v>683</v>
       </c>
       <c r="D9">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -844,7 +844,7 @@
         <v>683</v>
       </c>
       <c r="D10">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -888,7 +888,7 @@
         <v>683</v>
       </c>
       <c r="D11">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -932,7 +932,7 @@
         <v>683</v>
       </c>
       <c r="D12">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -976,7 +976,7 @@
         <v>683</v>
       </c>
       <c r="D13">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1020,7 +1020,7 @@
         <v>683</v>
       </c>
       <c r="D14">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -1064,7 +1064,7 @@
         <v>683</v>
       </c>
       <c r="D15">
-        <v>10129</v>
+        <v>10195</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>

</xml_diff>